<commit_message>
RM-32 códigos e updates
</commit_message>
<xml_diff>
--- a/05 - Execution/QR.xlsx
+++ b/05 - Execution/QR.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{75944EBC-A2A0-4F4D-B70C-21F8BDD78BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7573D06F-20F1-4C89-BC74-6ACB2181D390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,15 +29,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>Conteúdo</t>
-  </si>
-  <si>
-    <t>Código</t>
   </si>
   <si>
     <t>QR Code</t>
@@ -50,9 +44,6 @@
   </si>
   <si>
     <t>Peça A</t>
-  </si>
-  <si>
-    <t>Peça B</t>
   </si>
   <si>
     <t>Peça C</t>
@@ -110,6 +101,18 @@
   </si>
   <si>
     <t xml:space="preserve">    QR Codes </t>
+  </si>
+  <si>
+    <t>Código Caixa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Conteúdo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peça B   </t>
+  </si>
+  <si>
+    <t>Referência da Peça</t>
   </si>
 </sst>
 </file>
@@ -776,7 +779,7 @@
     <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -823,8 +826,14 @@
     <xf numFmtId="44" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="12"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="12"/>
@@ -832,12 +841,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="12"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Cor1" xfId="24" builtinId="30" customBuiltin="1"/>
@@ -888,7 +898,83 @@
     <cellStyle name="Verificar Célula" xfId="18" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="23">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -898,6 +984,43 @@
       <font>
         <color rgb="FFC00000"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14993743705557422"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -920,14 +1043,11 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
+        <right/>
         <top style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </top>
@@ -981,8 +1101,6 @@
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -996,20 +1114,22 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+          <bgColor theme="0"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
         <top style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
         </top>
         <bottom style="thin">
-          <color theme="0" tint="-0.14993743705557422"/>
+          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -1055,6 +1175,43 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -1087,77 +1244,6 @@
         </top>
         <bottom style="thin">
           <color theme="0" tint="-0.14993743705557422"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1" tint="0.34998626667073579"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </left>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <top style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </top>
-        <bottom style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </bottom>
       </border>
     </dxf>
@@ -1372,13 +1458,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="CollegeBudget2" pivot="0" count="7" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="22"/>
-      <tableStyleElement type="headerRow" dxfId="21"/>
-      <tableStyleElement type="totalRow" dxfId="20"/>
-      <tableStyleElement type="firstColumn" dxfId="19"/>
-      <tableStyleElement type="lastColumn" dxfId="18"/>
-      <tableStyleElement type="firstRowStripe" dxfId="17"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="lastColumn" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1394,6 +1480,65 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2552700</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1606550</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18" descr="2x Lego Duplo Basic Construction Stone Neu-Dunkel Grey 2x8 6157 9218 4971 |  eBay">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9A74734-4B4E-98EA-3BC4-680BB8130406}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="19086" b="14516"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5848350" y="9982200"/>
+          <a:ext cx="2381250" cy="1568450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1421,7 +1566,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1455,14 +1600,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>82550</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1968500</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1720850</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>1479550</xdr:rowOff>
     </xdr:to>
@@ -1472,56 +1617,6 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67127543-80DB-FD77-0A10-0B34A679FF99}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6464300" y="3409950"/>
-          <a:ext cx="1397000" cy="1397000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1955800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>1587500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Peça B">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA53DA3-A4C9-9343-2D10-F04F7FAD1C9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1543,8 +1638,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6375400" y="5092700"/>
-          <a:ext cx="1473200" cy="1473200"/>
+          <a:off x="8890000" y="3409950"/>
+          <a:ext cx="1397000" cy="1397000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1555,23 +1650,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>69850</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1949450</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1562100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1720850</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1587500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="12" name="Peça C">
+        <xdr:cNvPr id="10" name="Peça B">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2B95219-3046-F42A-3EB6-CC83F40FE804}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDA53DA3-A4C9-9343-2D10-F04F7FAD1C9D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1593,8 +1688,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6350000" y="6699250"/>
-          <a:ext cx="1492250" cy="1492250"/>
+          <a:off x="8813800" y="5092700"/>
+          <a:ext cx="1473200" cy="1473200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1605,23 +1700,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2012950</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1600200</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1758950</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1562100</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Peça D">
+        <xdr:cNvPr id="12" name="Peça C">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1716E25C-5ACD-65C2-B6C5-BA465C98C819}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2B95219-3046-F42A-3EB6-CC83F40FE804}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1643,8 +1738,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6330950" y="8312150"/>
-          <a:ext cx="1574800" cy="1574800"/>
+          <a:off x="8832850" y="6699250"/>
+          <a:ext cx="1492250" cy="1492250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1655,23 +1750,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>450850</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2032000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1593850</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1816100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1619250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="16" name="Peça E">
+        <xdr:cNvPr id="14" name="Peça D">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4589E8D6-A525-FF4F-16AC-562C4DF5D1E9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1716E25C-5ACD-65C2-B6C5-BA465C98C819}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1693,8 +1788,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6343650" y="9956800"/>
-          <a:ext cx="1581150" cy="1581150"/>
+          <a:off x="8807450" y="8331200"/>
+          <a:ext cx="1574800" cy="1574800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1705,23 +1800,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1993900</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1549400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1809750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1612900</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="18" name="Peça F">
+        <xdr:cNvPr id="16" name="Peça E">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C96F41-0876-BC3A-BCA6-CD3DE420E914}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4589E8D6-A525-FF4F-16AC-562C4DF5D1E9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1743,8 +1838,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6350000" y="11607800"/>
-          <a:ext cx="1536700" cy="1536700"/>
+          <a:off x="8794750" y="9975850"/>
+          <a:ext cx="1581150" cy="1581150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1755,23 +1850,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1955800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>1581150</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1765300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1549400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="20" name="Peça G">
+        <xdr:cNvPr id="18" name="Peça F">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896E9D64-2C00-BEE9-1AB5-A1AB9F5F3A31}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C96F41-0876-BC3A-BCA6-CD3DE420E914}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1793,8 +1888,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6292850" y="13252450"/>
-          <a:ext cx="1555750" cy="1555750"/>
+          <a:off x="8794750" y="11607800"/>
+          <a:ext cx="1536700" cy="1536700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1805,23 +1900,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2000250</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>1619250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>1581150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="22" name="Peça H">
+        <xdr:cNvPr id="20" name="Peça G">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52C6C461-1586-6447-2379-2CE6E39E02B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{896E9D64-2C00-BEE9-1AB5-A1AB9F5F3A31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1843,8 +1938,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6286500" y="14890750"/>
-          <a:ext cx="1606550" cy="1606550"/>
+          <a:off x="8782050" y="13252450"/>
+          <a:ext cx="1555750" cy="1555750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1855,23 +1950,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>387350</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2000250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1771650</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1619250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="24" name="Peça I">
+        <xdr:cNvPr id="22" name="Peça H">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E3878B-68D7-CED9-1B07-D02C2CD85A10}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52C6C461-1586-6447-2379-2CE6E39E02B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1893,8 +1988,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6280150" y="16560800"/>
-          <a:ext cx="1612900" cy="1612900"/>
+          <a:off x="8731250" y="14890750"/>
+          <a:ext cx="1606550" cy="1606550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1905,23 +2000,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1968500</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1758950</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="26" name="Peça J">
+        <xdr:cNvPr id="24" name="Peça I">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9652497-9BC2-21BF-E8B3-4DC9C51580DB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9E3878B-68D7-CED9-1B07-D02C2CD85A10}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1943,7 +2038,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6248400" y="18211800"/>
+          <a:off x="8712200" y="16560800"/>
           <a:ext cx="1612900" cy="1612900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1955,23 +2050,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1504951</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85726</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>1543050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1765300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="28" name="placa Verde">
+        <xdr:cNvPr id="26" name="Peça J">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13CE0531-34B3-A109-7829-A791DC32E124}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9652497-9BC2-21BF-E8B3-4DC9C51580DB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1993,8 +2088,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4121151" y="3413126"/>
-          <a:ext cx="1943099" cy="1457324"/>
+          <a:off x="8718550" y="18211800"/>
+          <a:ext cx="1612900" cy="1612900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2003,16 +2098,320 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1993900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1587500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6" descr="1 x Lego Duplo brick blue plate 8 x 8 with Trap Door Opening 51705">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F6B7A29-E5C9-9B83-7587-03B32A6F790E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6350000" y="5029200"/>
+          <a:ext cx="1536700" cy="1536700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>260350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2613358</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1492250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8" descr="LEGO® DUPLO PIASTRA di base Piastra di costruzione 8x16 16x8 VERDE CHIARO  EUR 7,30 - PicClick IT">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0F259F3-7F9E-22D5-7FD4-66A5A0297D73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="21600" b="13983"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5956300" y="3587750"/>
+          <a:ext cx="2549858" cy="1231900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>431800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>62260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2457450</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>1593849</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10" descr="Lego Duplo Bauplatte Platte 4x8 grau: Amazon.de: Spielzeug">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78F35FE7-AF78-5C17-8689-9EC3578E87FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6108700" y="6691660"/>
+          <a:ext cx="2025650" cy="1531589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>450850</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>82551</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2279650</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1635037</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagem 16" descr="Amazon.com: LEGO Parts and Pieces: DUPLO Bright Green 2x4 Brick x10 : Toys  &amp; Games">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD837F19-1AE8-79F3-C64B-9E4D60D6E5AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6127750" y="8369301"/>
+          <a:ext cx="1828800" cy="1552486"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>501854</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>133146</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1956210</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>1585501</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagem 28" descr="LEGO Part 3437 Duplo, Brick 2 x 2 [Dark Blue-Violet] (4221630) |  iBricktoys: LEGO shop guide and database">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7E8BED0-05BC-F6CF-2A78-035540AA0276}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6175886" y="11737259"/>
+          <a:ext cx="1454356" cy="1452355"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:E17" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" totalsRowDxfId="11" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="10">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Conteúdo" dataDxfId="9" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Código" dataDxfId="2" totalsRowDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="8" totalsRowDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="7" totalsRowDxfId="4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_AcademicExpenses" displayName="Table_AcademicExpenses" ref="B7:F17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" totalsRowDxfId="13" headerRowBorderDxfId="16" tableBorderDxfId="14" totalsRowBorderDxfId="12">
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Conteúdo " dataDxfId="11" totalsRowDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{3341B563-EB1E-48B1-94F1-39D1CCC81DB5}" name="Referência da Peça" dataDxfId="0" totalsRowDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Código Caixa" dataDxfId="9" totalsRowDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Peça" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="QR Code" dataDxfId="5" totalsRowDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2281,229 +2680,256 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:J37"/>
+  <dimension ref="B1:N37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="1.453125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36" style="1" customWidth="1"/>
+    <col min="2" max="2" width="32.90625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.453125" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.453125" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.26953125" style="1" customWidth="1"/>
-    <col min="6" max="10" width="1.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.453125" style="1" customWidth="1"/>
+    <col min="7" max="10" width="1.7265625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="19" t="s">
-        <v>26</v>
+    <row r="1" spans="2:14" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:14" customFormat="1" ht="94.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="18" t="s">
+        <v>23</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
       <c r="F2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="2:10" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:14" ht="10.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="11"/>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="2:10" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:14" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" spans="2:10" s="3" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="16" t="s">
+    <row r="6" spans="2:14" s="3" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+    </row>
+    <row r="7" spans="2:14" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-    </row>
-    <row r="7" spans="2:10" ht="48" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="13" t="s">
-        <v>1</v>
+      <c r="C8" s="21">
+        <v>6490</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>2</v>
+      <c r="D8" s="15" t="s">
+        <v>13</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="E8" s="23"/>
+      <c r="F8" s="8"/>
+      <c r="K8" s="16"/>
+    </row>
+    <row r="9" spans="2:14" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="21">
+        <v>51705</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="2:14" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>3</v>
+      <c r="C10" s="21">
+        <v>4672</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="7" t="s">
+      <c r="D10" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="2:14" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C11" s="21">
+        <v>3011</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="8"/>
-      <c r="J8" s="20"/>
-    </row>
-    <row r="9" spans="2:10" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="7" t="s">
+      <c r="E11"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="2:14" s="10" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C12" s="21">
+        <v>3007</v>
+      </c>
+      <c r="D12" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="8"/>
-    </row>
-    <row r="10" spans="2:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="7" t="s">
+      <c r="E12" s="23"/>
+      <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="2:14" s="3" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C13" s="21">
+        <v>3437</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="2:10" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="7" t="s">
+      <c r="E13"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" spans="2:14" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="15"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="2:10" s="10" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
+      <c r="E14" s="15"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="2:14" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="15"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="2:10" s="3" customFormat="1" ht="128.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="7" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="8"/>
+      <c r="N15" s="16"/>
+    </row>
+    <row r="16" spans="2:14" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="2:10" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="7" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="8"/>
+    </row>
+    <row r="17" spans="2:6" ht="130" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C17" s="7"/>
+      <c r="D17" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="2:10" ht="129.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" spans="2:10" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="2:5" ht="130" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="E17" s="15"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-    </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:5" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" s="10" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="2:5" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" s="3" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="2:5" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="16"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
-      <c r="E31" s="16"/>
-    </row>
-    <row r="32" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="17"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+    </row>
+    <row r="32" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:3" ht="18" customHeight="1" x14ac:dyDescent="0.35">
@@ -2543,22 +2969,22 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8:D17">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>D8&gt;C8</formula>
+  <conditionalFormatting sqref="E14:E17">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>E14&gt;D14</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="expression" dxfId="0" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>#REF!&gt;#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="8">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Orçamento Universitário Mensal" prompt="Este modelo monitoriza as suas despesas reais em relação ao seu orçamento universitário mensal._x000a__x000a_Introduzia os seus itens de despesa e orçamento nas três tabelas. Atualize a coluna Gastos Reais à medida que gasta dinheiro._x000a_" sqref="A2" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza Itens de Despesa abaixo desta coluna" sqref="B7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza o Orçamento por item sob esta coluna" sqref="C7" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza o Gasto Real por item sob esta coluna" sqref="D7" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduzir notas de itens abaixo sob esta coluna" sqref="E7" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza Itens de Despesa abaixo desta coluna" sqref="B7:C7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza o Orçamento por item sob esta coluna" sqref="D7" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduza o Gasto Real por item sob esta coluna" sqref="E7" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Introduzir notas de itens abaixo sob esta coluna" sqref="F7" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O Orçamento Total Mensal é calculado nesta célula" sqref="B5" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="O total dos gastos reais é calculado nesta célula" sqref="C5:D5" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Esta barra mostra a % do dinheiro gasto em relação ao orçamento total" sqref="E5" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
@@ -2597,26 +3023,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2904,6 +3310,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2914,18 +3340,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D95769C4-607B-4664-9C36-EC9F8E41992B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FE855E-B5B1-4D66-876A-F04E3BDA8A60}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2946,6 +3360,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D95769C4-607B-4664-9C36-EC9F8E41992B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{03FCA663-A0D5-4D37-87D6-2910454B74A5}">
   <ds:schemaRefs>

</xml_diff>